<commit_message>
removed ISRIC soil order variable from the Extra Info File
</commit_message>
<xml_diff>
--- a/Rpkg/inst/extdata/ISRaD_Extra_Info.xlsx
+++ b/Rpkg/inst/extdata/ISRaD_Extra_Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="0" windowWidth="21600" windowHeight="10820" tabRatio="500"/>
+    <workbookView xWindow="6460" yWindow="0" windowWidth="21600" windowHeight="10820" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="211">
   <si>
     <t>Units/Info</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>pro_PET</t>
-  </si>
-  <si>
-    <t>pro_ISRIC_USDA_250m</t>
   </si>
   <si>
     <t>Graven Radiocarbon Zone</t>
@@ -278,9 +275,6 @@
     <t>Potential evapotranspiration as calculated using Penman-Monteith method for short-clipped grass w/ worldclim input data. PET raster from: Kramer, M. and O. Chadwick. 2018. Climate-driven thresholds in reactive mineral retention of soil carbon at the global scale. Nature Climate Change 8:1104–1108.</t>
   </si>
   <si>
-    <t>USDA Soil Classification from 250 m resolution raster</t>
-  </si>
-  <si>
     <t>flx_graven_atm</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t>inc_dd14c</t>
   </si>
   <si>
-    <t>Soil Order in USDA Taxonomy</t>
-  </si>
-  <si>
     <t>Alfisols, Andisols, Aridisols, Entisols, Gelisols, Histosols, Inceptisols, Mollisols, Oxisols, Spodosols, Ultisols, Vertisols</t>
   </si>
   <si>
@@ -327,9 +318,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracts soil sub-order using global location from ISRIC gridded soil products. 250 meter spatial resolution. Grid cells classified as 'water' will produce empty values in this field. </t>
   </si>
   <si>
     <t>pro_0.5_landCover_MODIS</t>
@@ -780,18 +768,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1226,7 +1208,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1296,17 +1278,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2063,7 +2034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2075,18 +2046,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="93" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="92" customHeight="1">
-      <c r="A2" s="40" t="s">
-        <v>188</v>
+      <c r="A2" s="35" t="s">
+        <v>184</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2208,13 +2179,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2261,7 +2232,7 @@
         <v>16</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K1" s="28"/>
     </row>
@@ -2270,23 +2241,23 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2294,23 +2265,23 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2318,23 +2289,23 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2342,10 +2313,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
@@ -2355,7 +2326,7 @@
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2363,23 +2334,23 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2387,23 +2358,23 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2411,23 +2382,23 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2435,23 +2406,23 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2459,23 +2430,23 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2483,23 +2454,23 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2507,23 +2478,23 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2531,23 +2502,23 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2555,23 +2526,23 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2579,23 +2550,23 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2603,23 +2574,23 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2627,10 +2598,10 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="8"/>
       <c r="F17" t="s">
@@ -2638,7 +2609,7 @@
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2646,23 +2617,23 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2670,23 +2641,23 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2694,23 +2665,23 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2718,23 +2689,23 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2742,201 +2713,205 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="E22" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>17</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" s="36" customFormat="1">
-      <c r="A23" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="K23" s="37"/>
-    </row>
-    <row r="24" spans="1:11" ht="17" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>5</v>
+      <c r="E24" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>114</v>
+      <c r="F25" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>10</v>
+        <v>15000</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
+      <c r="D26" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>-60</v>
       </c>
       <c r="H26">
-        <v>15000</v>
+        <v>60</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B27" t="s">
-        <v>107</v>
+      <c r="F27" s="1" t="s">
+        <v>17</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>105</v>
+      <c r="I27" s="8" t="s">
+        <v>94</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>9</v>
+      <c r="J27" s="27" t="s">
+        <v>96</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>112</v>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1">
+      <c r="A28" s="29" t="s">
+        <v>113</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="B28" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G27">
-        <v>-60</v>
+      <c r="G28" s="24">
+        <v>0</v>
       </c>
-      <c r="H27">
-        <v>60</v>
+      <c r="H28" s="24">
+        <v>1000</v>
       </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="27" t="s">
-        <v>99</v>
+      <c r="I28" s="24"/>
+      <c r="J28" s="30" t="s">
+        <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J28" s="27" t="s">
-        <v>99</v>
-      </c>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1">
       <c r="A29" s="29" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>5</v>
@@ -2949,25 +2924,25 @@
       </c>
       <c r="I29" s="24"/>
       <c r="J29" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1">
       <c r="A30" s="29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>5</v>
@@ -2980,25 +2955,25 @@
       </c>
       <c r="I30" s="24"/>
       <c r="J30" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K30" s="24"/>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1">
       <c r="A31" s="29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C31" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>171</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>5</v>
@@ -3011,25 +2986,25 @@
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1">
       <c r="A32" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>5</v>
@@ -3042,25 +3017,25 @@
       </c>
       <c r="I32" s="24"/>
       <c r="J32" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1">
       <c r="A33" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>5</v>
@@ -3073,56 +3048,55 @@
       </c>
       <c r="I33" s="24"/>
       <c r="J33" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1">
-      <c r="A34" s="29" t="s">
-        <v>134</v>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1" t="s">
+        <v>120</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>107</v>
+      <c r="B34" t="s">
+        <v>103</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>170</v>
+      <c r="C34" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>171</v>
+        <v>2</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>164</v>
+      <c r="E34" s="8" t="s">
+        <v>175</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="F34" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34" s="24">
-        <v>1000</v>
+      <c r="H34">
+        <v>100</v>
       </c>
-      <c r="I34" s="24"/>
-      <c r="J34" s="30" t="s">
-        <v>99</v>
+      <c r="I34" s="8"/>
+      <c r="J34" s="27" t="s">
+        <v>96</v>
       </c>
-      <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
@@ -3135,24 +3109,24 @@
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="1" t="s">
-        <v>126</v>
+      <c r="A36" s="29" t="s">
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
@@ -3165,24 +3139,24 @@
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
@@ -3195,24 +3169,24 @@
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="29" t="s">
-        <v>129</v>
+      <c r="A38" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F38" t="s">
         <v>5</v>
@@ -3225,24 +3199,24 @@
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F39" t="s">
         <v>5</v>
@@ -3255,54 +3229,54 @@
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
-      <c r="D40" s="24" t="s">
-        <v>2</v>
+      <c r="D40" t="s">
+        <v>11</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>179</v>
+      <c r="E40" s="20" t="s">
+        <v>174</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>5</v>
@@ -3315,24 +3289,24 @@
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>5</v>
@@ -3345,24 +3319,24 @@
       </c>
       <c r="I42" s="8"/>
       <c r="J42" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>5</v>
@@ -3375,24 +3349,24 @@
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>5</v>
@@ -3405,24 +3379,24 @@
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -3435,24 +3409,24 @@
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>5</v>
@@ -3465,7 +3439,7 @@
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3473,16 +3447,16 @@
         <v>118</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>5</v>
@@ -3495,24 +3469,24 @@
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>5</v>
@@ -3525,24 +3499,24 @@
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>5</v>
@@ -3555,24 +3529,24 @@
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>5</v>
@@ -3585,24 +3559,24 @@
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>5</v>
@@ -3615,24 +3589,24 @@
       </c>
       <c r="I51" s="8"/>
       <c r="J51" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>5</v>
@@ -3645,24 +3619,24 @@
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>5</v>
@@ -3675,24 +3649,24 @@
       </c>
       <c r="I53" s="8"/>
       <c r="J53" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>5</v>
@@ -3705,24 +3679,24 @@
       </c>
       <c r="I54" s="8"/>
       <c r="J54" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>5</v>
@@ -3735,24 +3709,24 @@
       </c>
       <c r="I55" s="8"/>
       <c r="J55" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>5</v>
@@ -3765,37 +3739,7 @@
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57" t="s">
-        <v>107</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D57" t="s">
-        <v>135</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>1000</v>
-      </c>
-      <c r="I57" s="8"/>
-      <c r="J57" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3862,19 +3806,19 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -3888,19 +3832,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -4141,19 +4085,19 @@
     </row>
     <row r="2" spans="1:9" s="32" customFormat="1">
       <c r="A2" s="32" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -4167,19 +4111,19 @@
     </row>
     <row r="3" spans="1:9" s="20" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -4193,19 +4137,19 @@
     </row>
     <row r="4" spans="1:9" s="20" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>5</v>
@@ -4213,19 +4157,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="20" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F5" s="33" t="s">
         <v>5</v>
@@ -4239,19 +4183,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>5</v>
@@ -4261,19 +4205,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="20" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>5</v>
@@ -4287,19 +4231,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="20" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>5</v>
@@ -5606,19 +5550,19 @@
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -5633,19 +5577,19 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -71146,24 +71090,24 @@
         <v>16</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -71175,24 +71119,24 @@
         <v>1000</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -71204,7 +71148,7 @@
         <v>1000</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -71273,19 +71217,19 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1">
       <c r="A2" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>5</v>
@@ -71300,19 +71244,19 @@
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1">
       <c r="A3" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updated build fx with new read_xl package functions and updated geospatial files
</commit_message>
<xml_diff>
--- a/Rpkg/inst/extdata/ISRaD_Extra_Info.xlsx
+++ b/Rpkg/inst/extdata/ISRaD_Extra_Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="0" windowWidth="21600" windowHeight="10820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6460" yWindow="0" windowWidth="21600" windowHeight="15880" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="221">
   <si>
     <t>Units/Info</t>
   </si>
@@ -219,57 +219,6 @@
   </si>
   <si>
     <t>mm yr-1</t>
-  </si>
-  <si>
-    <t>Mean annual temperature from WorldClim</t>
-  </si>
-  <si>
-    <t>Average Day/Night Temperature range; max temp minus min temp</t>
-  </si>
-  <si>
-    <t>Variation in temperature over the course of a year, as calculated with standard deviation of MAT</t>
-  </si>
-  <si>
-    <t>Maximum temperature of hottest month (hottest temperature of the year)</t>
-  </si>
-  <si>
-    <t>Minimum temperature of coldest month (coldest temperature of the year)</t>
-  </si>
-  <si>
-    <t>Maximum temperature range during year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average temperature during wettest 3 consecutive months of the year </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average temperature during driest 3 consecutive months of the year </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average temperature during warmest 3 consecutive months of the year </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average temperature during coldest 3 consecutive months of the year </t>
-  </si>
-  <si>
-    <t>Mean annual precipitation</t>
-  </si>
-  <si>
-    <t>Precipitation during average wettest month of the year</t>
-  </si>
-  <si>
-    <t>Precipitation during average driest month of the year</t>
-  </si>
-  <si>
-    <t>Rainfall during 3 wettest months of the year</t>
-  </si>
-  <si>
-    <t>Rainfall during 3 driest months of the year</t>
-  </si>
-  <si>
-    <t>Rainfall during 3 warmest months of the year</t>
-  </si>
-  <si>
-    <t>Rainfall during 3 coldest months of the year</t>
   </si>
   <si>
     <t>Potential evapotranspiration as calculated using Penman-Monteith method for short-clipped grass w/ worldclim input data. PET raster from: Kramer, M. and O. Chadwick. 2018. Climate-driven thresholds in reactive mineral retention of soil carbon at the global scale. Nature Climate Change 8:1104–1108.</t>
@@ -661,6 +610,87 @@
   <si>
     <t>Most added data is filled at the profile and layer levels. More information about the fill functions can be retrieved from the documentation of the functions themselves. Data is of two types: calculated from exisiting data (e.g. lyr_soc_stock_filled), or filled from gridded global datasets (e.g. pro_SG_corg_10cm).</t>
   </si>
+  <si>
+    <t>from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Variation in temperature over the course of a year, as calculated with standard deviation of MAT, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Precipitation during average wettest month of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Precipitation during average driest month of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Rainfall during 3 wettest months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Rainfall during 3 driest months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Rainfall during 3 warmest months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Rainfall during 3 coldest months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Mean annual temperature, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Average Day/Night Temperature range; max temp minus min temp, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Maximum temperature of hottest month (hottest temperature of the year), from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Minimum temperature of coldest month (coldest temperature of the year), from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Maximum temperature range during year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Average temperature during wettest 3 consecutive months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Average temperature during driest 3 consecutive months of the yea,r from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Average temperature during warmest 3 consecutive months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Average temperature during coldest 3 consecutive months of the year, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>Mean annual precipitation, from WorldClim v2.1 (30" resolution)</t>
+  </si>
+  <si>
+    <t>pro_KG_future</t>
+  </si>
+  <si>
+    <t>pro_KG_present</t>
+  </si>
+  <si>
+    <t>Koeppen-Geiger Climate Predicted</t>
+  </si>
+  <si>
+    <t>Koeppen-Geiger Climate Present</t>
+  </si>
+  <si>
+    <t>Koeppen-Geiger climate classes for the period 1980-2016, 0.5 degree resolution (data from Beck et al. 2018, doi:10.1038/sdata.2018.214)</t>
+  </si>
+  <si>
+    <t>Koeppen-Geiger climate classes predicted for the future period 2071-2100, 0.5 degree resolution (data from Beck et al. 2018, doi:10.1038/sdata.2018.214)</t>
+  </si>
+  <si>
+    <t>pro_TC_soilMoist_mm</t>
+  </si>
+  <si>
+    <t>Soil Moisture</t>
+  </si>
+  <si>
+    <t>Estimated total column soil moisture in mm from TerraClim (Abatzoglou et al. 2018, doi.org/10.1038/sdata.2017.191), averaged over the period 1981-2010, at 2.5' resolution (ca. 4 km)</t>
+  </si>
 </sst>
 </file>
 
@@ -785,7 +815,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="421">
+  <cellStyleXfs count="429">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1207,6 +1237,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1282,7 +1320,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="421">
+  <cellStyles count="429">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1552,6 +1590,10 @@
     <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1698,6 +1740,10 @@
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="355"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="356"/>
@@ -2035,7 +2081,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2046,18 +2092,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="93" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="92" customHeight="1">
       <c r="A2" s="35" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2179,19 +2225,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="8" customWidth="1"/>
@@ -2232,7 +2278,7 @@
         <v>16</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="K1" s="28"/>
     </row>
@@ -2241,7 +2287,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>40</v>
@@ -2257,7 +2303,7 @@
         <v>42</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2265,7 +2311,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>43</v>
@@ -2274,14 +2320,14 @@
         <v>9</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2289,7 +2335,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>
@@ -2298,14 +2344,14 @@
         <v>9</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>65</v>
+        <v>203</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2313,7 +2359,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
@@ -2321,12 +2367,15 @@
       <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
+      <c r="E5" s="20" t="s">
+        <v>194</v>
+      </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2334,7 +2383,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>46</v>
@@ -2343,14 +2392,14 @@
         <v>9</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2358,7 +2407,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>47</v>
@@ -2367,14 +2416,14 @@
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2382,7 +2431,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>48</v>
@@ -2391,14 +2440,14 @@
         <v>9</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>68</v>
+        <v>205</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2406,7 +2455,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>49</v>
@@ -2415,14 +2464,14 @@
         <v>9</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>69</v>
+        <v>206</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2430,7 +2479,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>50</v>
@@ -2439,14 +2488,14 @@
         <v>9</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2454,7 +2503,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>51</v>
@@ -2463,14 +2512,14 @@
         <v>9</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2478,7 +2527,7 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>52</v>
@@ -2487,14 +2536,14 @@
         <v>9</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>72</v>
+        <v>209</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2502,7 +2551,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>53</v>
@@ -2511,14 +2560,14 @@
         <v>9</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>73</v>
+        <v>210</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2526,7 +2575,7 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>54</v>
@@ -2535,14 +2584,14 @@
         <v>63</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2550,7 +2599,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
@@ -2559,14 +2608,14 @@
         <v>10</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2574,7 +2623,7 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>56</v>
@@ -2583,14 +2632,14 @@
         <v>10</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>76</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2598,18 +2647,21 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="8"/>
+      <c r="E17" s="20" t="s">
+        <v>194</v>
+      </c>
       <c r="F17" t="s">
         <v>5</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2617,7 +2669,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>58</v>
@@ -2626,14 +2678,14 @@
         <v>10</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>77</v>
+        <v>198</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2641,7 +2693,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>59</v>
@@ -2650,14 +2702,14 @@
         <v>10</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2665,7 +2717,7 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>60</v>
@@ -2674,14 +2726,14 @@
         <v>10</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2689,7 +2741,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>61</v>
@@ -2698,14 +2750,14 @@
         <v>10</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2713,7 +2765,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>62</v>
@@ -2722,28 +2774,28 @@
         <v>63</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="17" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>5</v>
@@ -2756,21 +2808,21 @@
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2780,24 +2832,24 @@
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>5</v>
@@ -2810,24 +2862,24 @@
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>5</v>
@@ -2840,47 +2892,47 @@
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="J27" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1">
+      <c r="A28" s="29" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1">
-      <c r="A28" s="29" t="s">
-        <v>113</v>
-      </c>
       <c r="B28" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F28" s="29" t="s">
         <v>5</v>
@@ -2893,25 +2945,25 @@
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1">
       <c r="A29" s="29" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>5</v>
@@ -2924,25 +2976,25 @@
       </c>
       <c r="I29" s="24"/>
       <c r="J29" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1">
       <c r="A30" s="29" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F30" s="29" t="s">
         <v>5</v>
@@ -2955,25 +3007,25 @@
       </c>
       <c r="I30" s="24"/>
       <c r="J30" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K30" s="24"/>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1">
       <c r="A31" s="29" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>5</v>
@@ -2986,25 +3038,25 @@
       </c>
       <c r="I31" s="24"/>
       <c r="J31" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1">
       <c r="A32" s="29" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>5</v>
@@ -3017,25 +3069,25 @@
       </c>
       <c r="I32" s="24"/>
       <c r="J32" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1">
       <c r="A33" s="29" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F33" s="29" t="s">
         <v>5</v>
@@ -3048,25 +3100,25 @@
       </c>
       <c r="I33" s="24"/>
       <c r="J33" s="30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="K33" s="24"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F34" t="s">
         <v>5</v>
@@ -3079,24 +3131,24 @@
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
@@ -3109,24 +3161,24 @@
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="29" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
@@ -3139,24 +3191,24 @@
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="29" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
@@ -3169,24 +3221,24 @@
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F38" t="s">
         <v>5</v>
@@ -3199,24 +3251,24 @@
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F39" t="s">
         <v>5</v>
@@ -3229,24 +3281,24 @@
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>5</v>
@@ -3259,24 +3311,24 @@
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>5</v>
@@ -3289,24 +3341,24 @@
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>5</v>
@@ -3319,24 +3371,24 @@
       </c>
       <c r="I42" s="8"/>
       <c r="J42" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>5</v>
@@ -3349,24 +3401,24 @@
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>5</v>
@@ -3379,24 +3431,24 @@
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -3409,24 +3461,24 @@
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>5</v>
@@ -3439,24 +3491,24 @@
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>5</v>
@@ -3469,24 +3521,24 @@
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>5</v>
@@ -3499,24 +3551,24 @@
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>5</v>
@@ -3529,24 +3581,24 @@
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>5</v>
@@ -3559,24 +3611,24 @@
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>5</v>
@@ -3589,24 +3641,24 @@
       </c>
       <c r="I51" s="8"/>
       <c r="J51" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>5</v>
@@ -3619,24 +3671,24 @@
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>5</v>
@@ -3649,24 +3701,24 @@
       </c>
       <c r="I53" s="8"/>
       <c r="J53" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B54" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>5</v>
@@ -3679,24 +3731,24 @@
       </c>
       <c r="I54" s="8"/>
       <c r="J54" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>5</v>
@@ -3709,24 +3761,24 @@
       </c>
       <c r="I55" s="8"/>
       <c r="J55" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>5</v>
@@ -3739,7 +3791,58 @@
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="J57" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="J58" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3806,19 +3909,19 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -3832,19 +3935,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -4085,19 +4188,19 @@
     </row>
     <row r="2" spans="1:9" s="32" customFormat="1">
       <c r="A2" s="32" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -4111,19 +4214,19 @@
     </row>
     <row r="3" spans="1:9" s="20" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -4137,19 +4240,19 @@
     </row>
     <row r="4" spans="1:9" s="20" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>5</v>
@@ -4157,19 +4260,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="20" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="F5" s="33" t="s">
         <v>5</v>
@@ -4183,19 +4286,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="20" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>5</v>
@@ -4205,19 +4308,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="20" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>5</v>
@@ -4231,19 +4334,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="20" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>5</v>
@@ -5550,19 +5653,19 @@
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -5577,19 +5680,19 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -71090,24 +71193,24 @@
         <v>16</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -71119,24 +71222,24 @@
         <v>1000</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -71148,7 +71251,7 @@
         <v>1000</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -71217,19 +71320,19 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1">
       <c r="A2" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>103</v>
-      </c>
       <c r="C2" s="15" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>5</v>
@@ -71244,19 +71347,19 @@
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1">
       <c r="A3" s="25" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>5</v>

</xml_diff>